<commit_message>
Add files for dashboard from TQ
</commit_message>
<xml_diff>
--- a/BDOP_Holdings.xlsx
+++ b/BDOP_Holdings.xlsx
@@ -381,22 +381,22 @@
         <v>240423</v>
       </c>
       <c r="I2" s="63">
-        <v>3221288</v>
+        <v>3151836</v>
       </c>
       <c r="J2" s="56">
-        <v>0.049699999999999994</v>
+        <v>0.0481</v>
       </c>
       <c r="K2" s="63">
-        <v>3730551</v>
+        <v>3748770</v>
       </c>
       <c r="L2" s="66">
-        <v>15.52</v>
+        <v>15.59</v>
       </c>
       <c r="M2" s="66">
-        <v>13.40</v>
+        <v>13.11</v>
       </c>
       <c r="N2" s="56">
-        <v>-0.1365</v>
+        <v>-0.1592</v>
       </c>
       <c r="O2" s="56">
         <v>-0.0001</v>
@@ -442,16 +442,16 @@
     </row>
     <row r="3">
       <c r="A3" s="65">
-        <v>38598</v>
+        <v>16679</v>
       </c>
       <c t="inlineStr" r="B3">
         <is>
-          <t xml:space="preserve">Dave &amp; Buster'S Entertainment Inc.</t>
+          <t xml:space="preserve">Coty Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">PLAY US Equity</t>
+          <t xml:space="preserve">COTY US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D3">
@@ -461,7 +461,7 @@
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Consumer Staples</t>
         </is>
       </c>
       <c t="inlineStr" r="F3">
@@ -471,29 +471,29 @@
       </c>
       <c t="inlineStr" r="G3">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H3" s="63">
-        <v>57386</v>
+        <v>254449</v>
       </c>
       <c r="I3" s="63">
-        <v>2684582</v>
+        <v>2723949</v>
       </c>
       <c r="J3" s="56">
-        <v>0.0414</v>
+        <v>0.0416</v>
       </c>
       <c r="K3" s="63">
-        <v>2568063</v>
+        <v>2739753</v>
       </c>
       <c r="L3" s="66">
-        <v>44.75</v>
+        <v>10.77</v>
       </c>
       <c r="M3" s="66">
-        <v>46.78</v>
+        <v>10.71</v>
       </c>
       <c r="N3" s="56">
-        <v>0.0454</v>
+        <v>-0.0058</v>
       </c>
       <c r="O3" s="56">
         <v>0</v>
@@ -502,11 +502,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="65">
-        <v>238337109</v>
+        <v>222070203</v>
       </c>
       <c t="inlineStr" r="R3">
         <is>
-          <t xml:space="preserve">US2383371091</t>
+          <t xml:space="preserve">US2220702037</t>
         </is>
       </c>
       <c t="inlineStr" r="S3">
@@ -531,27 +531,27 @@
       </c>
       <c t="inlineStr" r="W3">
         <is>
-          <t xml:space="preserve">PLAY US Equity</t>
+          <t xml:space="preserve">COTY US Equity</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="65">
-        <v>38884</v>
+        <v>28169</v>
       </c>
       <c t="inlineStr" r="B4">
         <is>
-          <t xml:space="preserve">Accor Sa</t>
+          <t xml:space="preserve">Wynn Resorts Ltd.</t>
         </is>
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t xml:space="preserve">AC FP Equity</t>
+          <t xml:space="preserve">WYNN US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D4">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E4">
@@ -566,29 +566,29 @@
       </c>
       <c t="inlineStr" r="G4">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H4" s="63">
-        <v>60418</v>
+        <v>20612</v>
       </c>
       <c r="I4" s="63">
-        <v>2647149</v>
+        <v>2710746</v>
       </c>
       <c r="J4" s="56">
-        <v>0.0408</v>
+        <v>0.0414</v>
       </c>
       <c r="K4" s="63">
-        <v>2830668</v>
+        <v>2476651</v>
       </c>
       <c r="L4" s="66">
-        <v>46.85</v>
+        <v>120.16</v>
       </c>
       <c r="M4" s="66">
-        <v>43.81</v>
+        <v>131.51</v>
       </c>
       <c r="N4" s="56">
-        <v>-0.06480000000000001</v>
+        <v>0.09449999999999999</v>
       </c>
       <c r="O4" s="56">
         <v>0</v>
@@ -596,9 +596,12 @@
       <c t="n" r="P4">
         <v>0</v>
       </c>
+      <c r="Q4" s="65">
+        <v>983134107</v>
+      </c>
       <c t="inlineStr" r="R4">
         <is>
-          <t xml:space="preserve">FR0000120404</t>
+          <t xml:space="preserve">US9831341071</t>
         </is>
       </c>
       <c t="inlineStr" r="S4">
@@ -623,32 +626,32 @@
       </c>
       <c t="inlineStr" r="W4">
         <is>
-          <t xml:space="preserve">AC FP Equity</t>
+          <t xml:space="preserve">WYNN US Equity</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="65">
-        <v>16679</v>
+        <v>43255</v>
       </c>
       <c t="inlineStr" r="B5">
         <is>
-          <t xml:space="preserve">Coty Inc</t>
+          <t xml:space="preserve">Alsea Sab De Cv</t>
         </is>
       </c>
       <c t="inlineStr" r="C5">
         <is>
-          <t xml:space="preserve">COTY US Equity</t>
+          <t xml:space="preserve">ALSEA* MM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D5">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Mexico</t>
         </is>
       </c>
       <c t="inlineStr" r="E5">
         <is>
-          <t xml:space="preserve">Consumer Staples</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F5">
@@ -658,42 +661,44 @@
       </c>
       <c t="inlineStr" r="G5">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H5" s="63">
-        <v>254449</v>
+        <v>1024774</v>
       </c>
       <c r="I5" s="63">
-        <v>2637015</v>
+        <v>2673461</v>
       </c>
       <c r="J5" s="56">
-        <v>0.0407</v>
+        <v>0.0408</v>
       </c>
       <c r="K5" s="63">
-        <v>2726437</v>
+        <v>1663651</v>
       </c>
       <c r="L5" s="66">
-        <v>10.72</v>
+        <v>1.62</v>
       </c>
       <c r="M5" s="66">
-        <v>10.36</v>
+        <v>2.61</v>
       </c>
       <c r="N5" s="56">
-        <v>-0.032799999999999996</v>
+        <v>0.607</v>
       </c>
       <c r="O5" s="56">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c t="n" r="P5">
         <v>0</v>
       </c>
-      <c r="Q5" s="65">
-        <v>222070203</v>
+      <c t="inlineStr" r="Q5">
+        <is>
+          <t xml:space="preserve">P0212A104</t>
+        </is>
       </c>
       <c t="inlineStr" r="R5">
         <is>
-          <t xml:space="preserve">US2220702037</t>
+          <t xml:space="preserve">MXP001391012</t>
         </is>
       </c>
       <c t="inlineStr" r="S5">
@@ -718,27 +723,27 @@
       </c>
       <c t="inlineStr" r="W5">
         <is>
-          <t xml:space="preserve">COTY US Equity</t>
+          <t xml:space="preserve">ALSEA* MM Equity</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="65">
-        <v>38606</v>
+        <v>38884</v>
       </c>
       <c t="inlineStr" r="B6">
         <is>
-          <t xml:space="preserve">Dufry Ag</t>
+          <t xml:space="preserve">Accor Sa</t>
         </is>
       </c>
       <c t="inlineStr" r="C6">
         <is>
-          <t xml:space="preserve">DUFN SW Equity</t>
+          <t xml:space="preserve">AC FP Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D6">
         <is>
-          <t xml:space="preserve">Switzerland</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E6">
@@ -757,25 +762,25 @@
         </is>
       </c>
       <c r="H6" s="63">
-        <v>37494</v>
+        <v>60418</v>
       </c>
       <c r="I6" s="63">
-        <v>2629907</v>
+        <v>2603103</v>
       </c>
       <c r="J6" s="56">
-        <v>0.0406</v>
+        <v>0.0397</v>
       </c>
       <c r="K6" s="63">
-        <v>2757004</v>
+        <v>2858016</v>
       </c>
       <c r="L6" s="66">
-        <v>73.53</v>
+        <v>47.30</v>
       </c>
       <c r="M6" s="66">
-        <v>70.14</v>
+        <v>43.08</v>
       </c>
       <c r="N6" s="56">
-        <v>-0.0461</v>
+        <v>-0.0892</v>
       </c>
       <c r="O6" s="56">
         <v>0</v>
@@ -785,7 +790,7 @@
       </c>
       <c t="inlineStr" r="R6">
         <is>
-          <t xml:space="preserve">CH0023405456</t>
+          <t xml:space="preserve">FR0000120404</t>
         </is>
       </c>
       <c t="inlineStr" r="S6">
@@ -810,22 +815,22 @@
       </c>
       <c t="inlineStr" r="W6">
         <is>
-          <t xml:space="preserve">DUFN VX Equity</t>
+          <t xml:space="preserve">AC FP Equity</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="65">
-        <v>28169</v>
+        <v>49006</v>
       </c>
       <c t="inlineStr" r="B7">
         <is>
-          <t xml:space="preserve">Wynn Resorts Ltd.</t>
+          <t xml:space="preserve">Ke Holdings Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C7">
         <is>
-          <t xml:space="preserve">WYNN US Equity</t>
+          <t xml:space="preserve">BEKE US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D7">
@@ -835,7 +840,7 @@
       </c>
       <c t="inlineStr" r="E7">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Real Estate</t>
         </is>
       </c>
       <c t="inlineStr" r="F7">
@@ -849,25 +854,25 @@
         </is>
       </c>
       <c r="H7" s="63">
-        <v>20612</v>
+        <v>100570</v>
       </c>
       <c r="I7" s="63">
-        <v>2617369</v>
+        <v>2585949</v>
       </c>
       <c r="J7" s="56">
-        <v>0.0404</v>
+        <v>0.0395</v>
       </c>
       <c r="K7" s="63">
-        <v>2464615</v>
+        <v>2558985</v>
       </c>
       <c r="L7" s="66">
-        <v>119.57</v>
+        <v>25.44</v>
       </c>
       <c r="M7" s="66">
-        <v>126.98</v>
+        <v>25.71</v>
       </c>
       <c r="N7" s="56">
-        <v>0.062</v>
+        <v>0.0105</v>
       </c>
       <c r="O7" s="56">
         <v>0</v>
@@ -876,11 +881,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="65">
-        <v>983134107</v>
+        <v>482497104</v>
       </c>
       <c t="inlineStr" r="R7">
         <is>
-          <t xml:space="preserve">US9831341071</t>
+          <t xml:space="preserve">US4824971042</t>
         </is>
       </c>
       <c t="inlineStr" r="S7">
@@ -905,27 +910,27 @@
       </c>
       <c t="inlineStr" r="W7">
         <is>
-          <t xml:space="preserve">WYNN US Equity</t>
+          <t xml:space="preserve">BEKE US Equity</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="65">
-        <v>1248</v>
+        <v>38598</v>
       </c>
       <c t="inlineStr" r="B8">
         <is>
-          <t xml:space="preserve">Alibaba Group Holding Ltd</t>
+          <t xml:space="preserve">Dave &amp; Buster'S Entertainment Inc.</t>
         </is>
       </c>
       <c t="inlineStr" r="C8">
         <is>
-          <t xml:space="preserve">BABA US Equity</t>
+          <t xml:space="preserve">PLAY US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D8">
         <is>
-          <t xml:space="preserve">China</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E8">
@@ -940,44 +945,42 @@
       </c>
       <c t="inlineStr" r="G8">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H8" s="63">
-        <v>11790</v>
+        <v>57386</v>
       </c>
       <c r="I8" s="63">
-        <v>2510553</v>
+        <v>2573520</v>
       </c>
       <c r="J8" s="56">
-        <v>0.0387</v>
+        <v>0.0393</v>
       </c>
       <c r="K8" s="63">
-        <v>2989155</v>
+        <v>2580605</v>
       </c>
       <c r="L8" s="66">
-        <v>253.53</v>
+        <v>44.97</v>
       </c>
       <c r="M8" s="66">
-        <v>212.94</v>
+        <v>44.85</v>
       </c>
       <c r="N8" s="56">
-        <v>-0.16010000000000002</v>
+        <v>-0.0027</v>
       </c>
       <c r="O8" s="56">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c t="n" r="P8">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q8">
-        <is>
-          <t xml:space="preserve">01609W102</t>
-        </is>
+      <c r="Q8" s="65">
+        <v>238337109</v>
       </c>
       <c t="inlineStr" r="R8">
         <is>
-          <t xml:space="preserve">US01609W1027</t>
+          <t xml:space="preserve">US2383371091</t>
         </is>
       </c>
       <c t="inlineStr" r="S8">
@@ -1002,27 +1005,27 @@
       </c>
       <c t="inlineStr" r="W8">
         <is>
-          <t xml:space="preserve">EQ0000000035266994 Equity</t>
+          <t xml:space="preserve">PLAY US Equity</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="65">
-        <v>43255</v>
+        <v>1248</v>
       </c>
       <c t="inlineStr" r="B9">
         <is>
-          <t xml:space="preserve">Alsea Sab De Cv</t>
+          <t xml:space="preserve">Alibaba Group Holding Ltd</t>
         </is>
       </c>
       <c t="inlineStr" r="C9">
         <is>
-          <t xml:space="preserve">ALSEA* MM Equity</t>
+          <t xml:space="preserve">BABA US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D9">
         <is>
-          <t xml:space="preserve">Mexico</t>
+          <t xml:space="preserve">China</t>
         </is>
       </c>
       <c t="inlineStr" r="E9">
@@ -1037,44 +1040,44 @@
       </c>
       <c t="inlineStr" r="G9">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H9" s="63">
-        <v>1024774</v>
+        <v>11790</v>
       </c>
       <c r="I9" s="63">
-        <v>2510361</v>
+        <v>2496258</v>
       </c>
       <c r="J9" s="56">
-        <v>0.0387</v>
+        <v>0.0381</v>
       </c>
       <c r="K9" s="63">
-        <v>1629163</v>
+        <v>3003754</v>
       </c>
       <c r="L9" s="66">
-        <v>1.59</v>
+        <v>254.77</v>
       </c>
       <c r="M9" s="66">
-        <v>2.45</v>
+        <v>211.73</v>
       </c>
       <c r="N9" s="56">
-        <v>0.5409</v>
+        <v>-0.16899999999999998</v>
       </c>
       <c r="O9" s="56">
-        <v>0.0001</v>
+        <v>-0.0001</v>
       </c>
       <c t="n" r="P9">
         <v>0</v>
       </c>
       <c t="inlineStr" r="Q9">
         <is>
-          <t xml:space="preserve">P0212A104</t>
+          <t xml:space="preserve">01609W102</t>
         </is>
       </c>
       <c t="inlineStr" r="R9">
         <is>
-          <t xml:space="preserve">MXP001391012</t>
+          <t xml:space="preserve">US01609W1027</t>
         </is>
       </c>
       <c t="inlineStr" r="S9">
@@ -1099,22 +1102,22 @@
       </c>
       <c t="inlineStr" r="W9">
         <is>
-          <t xml:space="preserve">ALSEA* MM Equity</t>
+          <t xml:space="preserve">EQ0000000035266994 Equity</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="65">
-        <v>40359</v>
+        <v>45110</v>
       </c>
       <c t="inlineStr" r="B10">
         <is>
-          <t xml:space="preserve">Realreal Inc. (The)</t>
+          <t xml:space="preserve">Tal Education Group, Adr</t>
         </is>
       </c>
       <c t="inlineStr" r="C10">
         <is>
-          <t xml:space="preserve">REAL US Equity</t>
+          <t xml:space="preserve">TAL US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D10">
@@ -1138,40 +1141,38 @@
         </is>
       </c>
       <c r="H10" s="63">
-        <v>150054</v>
+        <v>362770</v>
       </c>
       <c r="I10" s="63">
-        <v>2441305</v>
+        <v>2478865</v>
       </c>
       <c r="J10" s="56">
-        <v>0.0377</v>
+        <v>0.0378</v>
       </c>
       <c r="K10" s="63">
-        <v>3527998</v>
+        <v>7531563</v>
       </c>
       <c r="L10" s="66">
-        <v>23.51</v>
+        <v>20.76</v>
       </c>
       <c r="M10" s="66">
-        <v>16.27</v>
+        <v>6.83</v>
       </c>
       <c r="N10" s="56">
-        <v>-0.308</v>
+        <v>-0.6709</v>
       </c>
       <c r="O10" s="56">
-        <v>-0.0001</v>
+        <v>-0.0007000000000000001</v>
       </c>
       <c t="n" r="P10">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q10">
-        <is>
-          <t xml:space="preserve">88339P101</t>
-        </is>
+      <c r="Q10" s="65">
+        <v>874080104</v>
       </c>
       <c t="inlineStr" r="R10">
         <is>
-          <t xml:space="preserve">US88339P1012</t>
+          <t xml:space="preserve">US8740801043</t>
         </is>
       </c>
       <c t="inlineStr" r="S10">
@@ -1196,22 +1197,22 @@
       </c>
       <c t="inlineStr" r="W10">
         <is>
-          <t xml:space="preserve">REAL US Equity</t>
+          <t xml:space="preserve">TAL US Equity</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="65">
-        <v>49006</v>
+        <v>40359</v>
       </c>
       <c t="inlineStr" r="B11">
         <is>
-          <t xml:space="preserve">Ke Holdings Inc</t>
+          <t xml:space="preserve">Realreal Inc. (The)</t>
         </is>
       </c>
       <c t="inlineStr" r="C11">
         <is>
-          <t xml:space="preserve">BEKE US Equity</t>
+          <t xml:space="preserve">REAL US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D11">
@@ -1221,7 +1222,7 @@
       </c>
       <c t="inlineStr" r="E11">
         <is>
-          <t xml:space="preserve">Real Estate</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F11">
@@ -1235,38 +1236,40 @@
         </is>
       </c>
       <c r="H11" s="63">
-        <v>100570</v>
+        <v>150054</v>
       </c>
       <c r="I11" s="63">
-        <v>2401147</v>
+        <v>2396265</v>
       </c>
       <c r="J11" s="56">
-        <v>0.037000000000000005</v>
+        <v>0.0366</v>
       </c>
       <c r="K11" s="63">
-        <v>2546548</v>
+        <v>3545228</v>
       </c>
       <c r="L11" s="66">
-        <v>25.32</v>
+        <v>23.63</v>
       </c>
       <c r="M11" s="66">
-        <v>23.88</v>
+        <v>15.97</v>
       </c>
       <c r="N11" s="56">
-        <v>-0.0571</v>
+        <v>-0.32409999999999994</v>
       </c>
       <c r="O11" s="56">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c t="n" r="P11">
         <v>0</v>
       </c>
-      <c r="Q11" s="65">
-        <v>482497104</v>
+      <c t="inlineStr" r="Q11">
+        <is>
+          <t xml:space="preserve">88339P101</t>
+        </is>
       </c>
       <c t="inlineStr" r="R11">
         <is>
-          <t xml:space="preserve">US4824971042</t>
+          <t xml:space="preserve">US88339P1012</t>
         </is>
       </c>
       <c t="inlineStr" r="S11">
@@ -1291,27 +1294,27 @@
       </c>
       <c t="inlineStr" r="W11">
         <is>
-          <t xml:space="preserve">BEKE US Equity</t>
+          <t xml:space="preserve">REAL US Equity</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="65">
-        <v>45110</v>
+        <v>38606</v>
       </c>
       <c t="inlineStr" r="B12">
         <is>
-          <t xml:space="preserve">Tal Education Group, Adr</t>
+          <t xml:space="preserve">Dufry Ag</t>
         </is>
       </c>
       <c t="inlineStr" r="C12">
         <is>
-          <t xml:space="preserve">TAL US Equity</t>
+          <t xml:space="preserve">DUFN SW Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D12">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Switzerland</t>
         </is>
       </c>
       <c t="inlineStr" r="E12">
@@ -1326,42 +1329,39 @@
       </c>
       <c t="inlineStr" r="G12">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H12" s="63">
-        <v>362770</v>
+        <v>37494</v>
       </c>
       <c r="I12" s="63">
-        <v>2370886</v>
+        <v>2394759</v>
       </c>
       <c r="J12" s="56">
         <v>0.0366</v>
       </c>
       <c r="K12" s="63">
-        <v>7494959</v>
+        <v>2761704</v>
       </c>
       <c r="L12" s="66">
-        <v>20.66</v>
+        <v>73.66</v>
       </c>
       <c r="M12" s="66">
-        <v>6.54</v>
+        <v>63.87</v>
       </c>
       <c r="N12" s="56">
-        <v>-0.6837000000000001</v>
+        <v>-0.1329</v>
       </c>
       <c r="O12" s="56">
-        <v>-0.0007000000000000001</v>
+        <v>-0.0001</v>
       </c>
       <c t="n" r="P12">
         <v>0</v>
       </c>
-      <c r="Q12" s="65">
-        <v>874080104</v>
-      </c>
       <c t="inlineStr" r="R12">
         <is>
-          <t xml:space="preserve">US8740801043</t>
+          <t xml:space="preserve">CH0023405456</t>
         </is>
       </c>
       <c t="inlineStr" r="S12">
@@ -1386,32 +1386,32 @@
       </c>
       <c t="inlineStr" r="W12">
         <is>
-          <t xml:space="preserve">TAL US Equity</t>
+          <t xml:space="preserve">DUFN VX Equity</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="65">
-        <v>8718</v>
+        <v>48513</v>
       </c>
       <c t="inlineStr" r="B13">
         <is>
-          <t xml:space="preserve">Atlantia Spa</t>
+          <t xml:space="preserve">Madison Square Garden Entertainment Corp</t>
         </is>
       </c>
       <c t="inlineStr" r="C13">
         <is>
-          <t xml:space="preserve">ATL IM Equity</t>
+          <t xml:space="preserve">MSGE US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D13">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E13">
         <is>
-          <t xml:space="preserve">Utilities</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F13">
@@ -1421,29 +1421,29 @@
       </c>
       <c t="inlineStr" r="G13">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H13" s="63">
-        <v>94968</v>
+        <v>23407</v>
       </c>
       <c r="I13" s="63">
-        <v>2242336</v>
+        <v>2317111</v>
       </c>
       <c r="J13" s="56">
-        <v>0.0346</v>
+        <v>0.0354</v>
       </c>
       <c r="K13" s="63">
-        <v>2234420</v>
+        <v>2114448</v>
       </c>
       <c r="L13" s="66">
-        <v>23.53</v>
+        <v>90.33</v>
       </c>
       <c r="M13" s="66">
-        <v>23.61</v>
+        <v>98.99</v>
       </c>
       <c r="N13" s="56">
-        <v>0.0034999999999999996</v>
+        <v>0.0958</v>
       </c>
       <c r="O13" s="56">
         <v>0</v>
@@ -1451,9 +1451,14 @@
       <c t="n" r="P13">
         <v>0</v>
       </c>
+      <c t="inlineStr" r="Q13">
+        <is>
+          <t xml:space="preserve">55826T102</t>
+        </is>
+      </c>
       <c t="inlineStr" r="R13">
         <is>
-          <t xml:space="preserve">IT0003506190</t>
+          <t xml:space="preserve">US55826T1025</t>
         </is>
       </c>
       <c t="inlineStr" r="S13">
@@ -1478,7 +1483,7 @@
       </c>
       <c t="inlineStr" r="W13">
         <is>
-          <t xml:space="preserve">IT0003506190 Equity</t>
+          <t xml:space="preserve">MSGE US Equity</t>
         </is>
       </c>
     </row>
@@ -1520,22 +1525,22 @@
         <v>166219</v>
       </c>
       <c r="I14" s="63">
-        <v>2234579</v>
+        <v>2270098</v>
       </c>
       <c r="J14" s="56">
-        <v>0.0345</v>
+        <v>0.0347</v>
       </c>
       <c r="K14" s="63">
-        <v>2437191</v>
+        <v>2460737</v>
       </c>
       <c r="L14" s="66">
-        <v>14.66</v>
+        <v>14.80</v>
       </c>
       <c r="M14" s="66">
-        <v>13.44</v>
+        <v>13.66</v>
       </c>
       <c r="N14" s="56">
-        <v>-0.08310000000000001</v>
+        <v>-0.0775</v>
       </c>
       <c r="O14" s="56">
         <v>0</v>
@@ -1581,26 +1586,26 @@
     </row>
     <row r="15">
       <c r="A15" s="65">
-        <v>48513</v>
+        <v>25528</v>
       </c>
       <c t="inlineStr" r="B15">
         <is>
-          <t xml:space="preserve">Madison Square Garden Entertainment Corp</t>
+          <t xml:space="preserve">Amadeus IT Holding SA</t>
         </is>
       </c>
       <c t="inlineStr" r="C15">
         <is>
-          <t xml:space="preserve">MSGE US Equity</t>
+          <t xml:space="preserve">AMS SM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D15">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E15">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Information Technology</t>
         </is>
       </c>
       <c t="inlineStr" r="F15">
@@ -1610,29 +1615,29 @@
       </c>
       <c t="inlineStr" r="G15">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H15" s="63">
-        <v>23407</v>
+        <v>28466</v>
       </c>
       <c r="I15" s="63">
-        <v>2207697</v>
+        <v>2268025</v>
       </c>
       <c r="J15" s="56">
-        <v>0.0341</v>
+        <v>0.0346</v>
       </c>
       <c r="K15" s="63">
-        <v>2104171</v>
+        <v>2478769</v>
       </c>
       <c r="L15" s="66">
-        <v>89.89</v>
+        <v>87.08</v>
       </c>
       <c r="M15" s="66">
-        <v>94.32</v>
+        <v>79.67</v>
       </c>
       <c r="N15" s="56">
-        <v>0.0492</v>
+        <v>-0.085</v>
       </c>
       <c r="O15" s="56">
         <v>0</v>
@@ -1640,14 +1645,9 @@
       <c t="n" r="P15">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q15">
-        <is>
-          <t xml:space="preserve">55826T102</t>
-        </is>
-      </c>
       <c t="inlineStr" r="R15">
         <is>
-          <t xml:space="preserve">US55826T1025</t>
+          <t xml:space="preserve">ES0109067019</t>
         </is>
       </c>
       <c t="inlineStr" r="S15">
@@ -1672,27 +1672,27 @@
       </c>
       <c t="inlineStr" r="W15">
         <is>
-          <t xml:space="preserve">MSGE US Equity</t>
+          <t xml:space="preserve">ES0109067019 Equity</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="65">
-        <v>25528</v>
+        <v>49547</v>
       </c>
       <c t="inlineStr" r="B16">
         <is>
-          <t xml:space="preserve">Amadeus IT Holding SA</t>
+          <t xml:space="preserve">Kingsoft Cloud Holdings Ltd</t>
         </is>
       </c>
       <c t="inlineStr" r="C16">
         <is>
-          <t xml:space="preserve">AMS SM Equity</t>
+          <t xml:space="preserve">KC US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D16">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E16">
@@ -1707,29 +1707,29 @@
       </c>
       <c t="inlineStr" r="G16">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H16" s="63">
-        <v>28466</v>
+        <v>52936</v>
       </c>
       <c r="I16" s="63">
-        <v>2177127</v>
+        <v>2263430</v>
       </c>
       <c r="J16" s="56">
-        <v>0.0336</v>
+        <v>0.0346</v>
       </c>
       <c r="K16" s="63">
-        <v>2455050</v>
+        <v>1923608</v>
       </c>
       <c r="L16" s="66">
-        <v>86.24</v>
+        <v>36.34</v>
       </c>
       <c r="M16" s="66">
-        <v>76.48</v>
+        <v>42.76</v>
       </c>
       <c r="N16" s="56">
-        <v>-0.11320000000000001</v>
+        <v>0.17670000000000002</v>
       </c>
       <c r="O16" s="56">
         <v>0</v>
@@ -1737,9 +1737,14 @@
       <c t="n" r="P16">
         <v>0</v>
       </c>
+      <c t="inlineStr" r="Q16">
+        <is>
+          <t xml:space="preserve">49639K101</t>
+        </is>
+      </c>
       <c t="inlineStr" r="R16">
         <is>
-          <t xml:space="preserve">ES0109067019</t>
+          <t xml:space="preserve">US49639K1016</t>
         </is>
       </c>
       <c t="inlineStr" r="S16">
@@ -1764,32 +1769,32 @@
       </c>
       <c t="inlineStr" r="W16">
         <is>
-          <t xml:space="preserve">ES0109067019 Equity</t>
+          <t xml:space="preserve">KC US Equity</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="65">
-        <v>13294</v>
+        <v>22571</v>
       </c>
       <c t="inlineStr" r="B17">
         <is>
-          <t xml:space="preserve">TENCENT HOLDINGS LTD</t>
+          <t xml:space="preserve">Prosus Nv</t>
         </is>
       </c>
       <c t="inlineStr" r="C17">
         <is>
-          <t xml:space="preserve">TCEHY US Equity</t>
+          <t xml:space="preserve">PROSF Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D17">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E17">
         <is>
-          <t xml:space="preserve">Communication Services</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F17">
@@ -1803,25 +1808,25 @@
         </is>
       </c>
       <c r="H17" s="63">
-        <v>28166</v>
+        <v>20257</v>
       </c>
       <c r="I17" s="63">
-        <v>2159649</v>
+        <v>2254835</v>
       </c>
       <c r="J17" s="56">
-        <v>0.0333</v>
+        <v>0.0344</v>
       </c>
       <c r="K17" s="63">
-        <v>2050517</v>
+        <v>2060931</v>
       </c>
       <c r="L17" s="66">
-        <v>72.80</v>
+        <v>101.74</v>
       </c>
       <c r="M17" s="66">
-        <v>76.68</v>
+        <v>111.31</v>
       </c>
       <c r="N17" s="56">
-        <v>0.053200000000000004</v>
+        <v>0.0941</v>
       </c>
       <c r="O17" s="56">
         <v>0</v>
@@ -1829,14 +1834,9 @@
       <c t="n" r="P17">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q17">
-        <is>
-          <t xml:space="preserve">88032Q109</t>
-        </is>
-      </c>
       <c t="inlineStr" r="R17">
         <is>
-          <t xml:space="preserve">US88032Q1094</t>
+          <t xml:space="preserve">NL0013654783</t>
         </is>
       </c>
       <c t="inlineStr" r="S17">
@@ -1861,32 +1861,32 @@
       </c>
       <c t="inlineStr" r="W17">
         <is>
-          <t xml:space="preserve">B3F2DZ7 US Equity</t>
+          <t xml:space="preserve">NL0013654783 Equity</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="65">
-        <v>22571</v>
+        <v>13294</v>
       </c>
       <c t="inlineStr" r="B18">
         <is>
-          <t xml:space="preserve">Prosus Nv</t>
+          <t xml:space="preserve">TENCENT HOLDINGS LTD</t>
         </is>
       </c>
       <c t="inlineStr" r="C18">
         <is>
-          <t xml:space="preserve">PROSF Equity</t>
+          <t xml:space="preserve">TCEHY US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D18">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E18">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Communication Services</t>
         </is>
       </c>
       <c t="inlineStr" r="F18">
@@ -1900,25 +1900,25 @@
         </is>
       </c>
       <c r="H18" s="63">
-        <v>20257</v>
+        <v>28166</v>
       </c>
       <c r="I18" s="63">
-        <v>2150089</v>
+        <v>2254666</v>
       </c>
       <c r="J18" s="56">
-        <v>0.0332</v>
+        <v>0.0344</v>
       </c>
       <c r="K18" s="63">
-        <v>2041210</v>
+        <v>2060531</v>
       </c>
       <c r="L18" s="66">
-        <v>100.77</v>
+        <v>73.16</v>
       </c>
       <c r="M18" s="66">
-        <v>106.14</v>
+        <v>80.05</v>
       </c>
       <c r="N18" s="56">
-        <v>0.0533</v>
+        <v>0.0942</v>
       </c>
       <c r="O18" s="56">
         <v>0</v>
@@ -1926,9 +1926,14 @@
       <c t="n" r="P18">
         <v>0</v>
       </c>
+      <c t="inlineStr" r="Q18">
+        <is>
+          <t xml:space="preserve">88032Q109</t>
+        </is>
+      </c>
       <c t="inlineStr" r="R18">
         <is>
-          <t xml:space="preserve">NL0013654783</t>
+          <t xml:space="preserve">US88032Q1094</t>
         </is>
       </c>
       <c t="inlineStr" r="S18">
@@ -1953,32 +1958,32 @@
       </c>
       <c t="inlineStr" r="W18">
         <is>
-          <t xml:space="preserve">NL0013654783 Equity</t>
+          <t xml:space="preserve">B3F2DZ7 US Equity</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="65">
-        <v>47562</v>
+        <v>8718</v>
       </c>
       <c t="inlineStr" r="B19">
         <is>
-          <t xml:space="preserve">Cielo Sa</t>
+          <t xml:space="preserve">Atlantia Spa</t>
         </is>
       </c>
       <c t="inlineStr" r="C19">
         <is>
-          <t xml:space="preserve">CIEL3 BZ Equity</t>
+          <t xml:space="preserve">ATL IM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D19">
         <is>
-          <t xml:space="preserve">Brazil</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E19">
         <is>
-          <t xml:space="preserve">Information Technology</t>
+          <t xml:space="preserve">Utilities</t>
         </is>
       </c>
       <c t="inlineStr" r="F19">
@@ -1988,44 +1993,39 @@
       </c>
       <c t="inlineStr" r="G19">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H19" s="63">
-        <v>2881500</v>
+        <v>94968</v>
       </c>
       <c r="I19" s="63">
-        <v>2082080</v>
+        <v>2244814</v>
       </c>
       <c r="J19" s="56">
-        <v>0.0321</v>
+        <v>0.034300000000000004</v>
       </c>
       <c r="K19" s="63">
-        <v>2783229</v>
+        <v>2256008</v>
       </c>
       <c r="L19" s="66">
-        <v>0.97</v>
+        <v>23.76</v>
       </c>
       <c r="M19" s="66">
-        <v>0.72</v>
+        <v>23.64</v>
       </c>
       <c r="N19" s="56">
-        <v>-0.2519</v>
+        <v>-0.005</v>
       </c>
       <c r="O19" s="56">
-        <v>-0.0001</v>
+        <v>0</v>
       </c>
       <c t="n" r="P19">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q19">
-        <is>
-          <t xml:space="preserve">P2859E100</t>
-        </is>
-      </c>
       <c t="inlineStr" r="R19">
         <is>
-          <t xml:space="preserve">BRCIELACNOR3</t>
+          <t xml:space="preserve">IT0003506190</t>
         </is>
       </c>
       <c t="inlineStr" r="S19">
@@ -2050,22 +2050,22 @@
       </c>
       <c t="inlineStr" r="W19">
         <is>
-          <t xml:space="preserve">CIEL3 BZ Equity</t>
+          <t xml:space="preserve">IT0003506190 Equity</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="65">
-        <v>48370</v>
+        <v>49005</v>
       </c>
       <c t="inlineStr" r="B20">
         <is>
-          <t xml:space="preserve">Irhythm Technologies Inc.</t>
+          <t xml:space="preserve">Autohome Inc., Adr</t>
         </is>
       </c>
       <c t="inlineStr" r="C20">
         <is>
-          <t xml:space="preserve">IRTC US Equity</t>
+          <t xml:space="preserve">ATHM US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D20">
@@ -2075,7 +2075,7 @@
       </c>
       <c t="inlineStr" r="E20">
         <is>
-          <t xml:space="preserve">Health Care</t>
+          <t xml:space="preserve">Communication Services</t>
         </is>
       </c>
       <c t="inlineStr" r="F20">
@@ -2089,25 +2089,25 @@
         </is>
       </c>
       <c r="H20" s="63">
-        <v>34924</v>
+        <v>38396</v>
       </c>
       <c r="I20" s="63">
-        <v>2034864</v>
+        <v>2237399</v>
       </c>
       <c r="J20" s="56">
-        <v>0.031400000000000004</v>
+        <v>0.0342</v>
       </c>
       <c r="K20" s="63">
-        <v>2326971</v>
+        <v>2053257</v>
       </c>
       <c r="L20" s="66">
-        <v>66.63</v>
+        <v>53.48</v>
       </c>
       <c r="M20" s="66">
         <v>58.27</v>
       </c>
       <c r="N20" s="56">
-        <v>-0.1255</v>
+        <v>0.0897</v>
       </c>
       <c r="O20" s="56">
         <v>0</v>
@@ -2115,12 +2115,14 @@
       <c t="n" r="P20">
         <v>0</v>
       </c>
-      <c r="Q20" s="65">
-        <v>450056106</v>
+      <c t="inlineStr" r="Q20">
+        <is>
+          <t xml:space="preserve">05278C107</t>
+        </is>
       </c>
       <c t="inlineStr" r="R20">
         <is>
-          <t xml:space="preserve">US4500561067</t>
+          <t xml:space="preserve">US05278C1071</t>
         </is>
       </c>
       <c t="inlineStr" r="S20">
@@ -2145,22 +2147,22 @@
       </c>
       <c t="inlineStr" r="W20">
         <is>
-          <t xml:space="preserve">IRTC US Equity</t>
+          <t xml:space="preserve">ATHM US Equity</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="65">
-        <v>38802</v>
+        <v>49848</v>
       </c>
       <c t="inlineStr" r="B21">
         <is>
-          <t xml:space="preserve">Sabre Corporation</t>
+          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 440 10/15/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C21">
         <is>
-          <t xml:space="preserve">SABR US Equity</t>
+          <t xml:space="preserve">SPY US 10/15/21 P440 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D21">
@@ -2170,39 +2172,39 @@
       </c>
       <c t="inlineStr" r="E21">
         <is>
-          <t xml:space="preserve">Information Technology</t>
+          <t xml:space="preserve">Equity Index</t>
         </is>
       </c>
       <c t="inlineStr" r="F21">
         <is>
-          <t xml:space="preserve">Equity</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c t="inlineStr" r="G21">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c r="H21" s="63">
-        <v>146057</v>
+        <v>3000</v>
       </c>
       <c r="I21" s="63">
-        <v>2030502</v>
+        <v>2194204</v>
       </c>
       <c r="J21" s="56">
-        <v>0.0313</v>
+        <v>0.0335</v>
       </c>
       <c r="K21" s="63">
-        <v>2293786</v>
+        <v>2085427</v>
       </c>
       <c r="L21" s="66">
-        <v>15.70</v>
+        <v>6.95</v>
       </c>
       <c r="M21" s="66">
-        <v>13.90</v>
+        <v>7.31</v>
       </c>
       <c r="N21" s="56">
-        <v>-0.1148</v>
+        <v>0.052199999999999996</v>
       </c>
       <c r="O21" s="56">
         <v>0</v>
@@ -2210,14 +2212,9 @@
       <c t="n" r="P21">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q21">
-        <is>
-          <t xml:space="preserve">78573M104</t>
-        </is>
-      </c>
       <c t="inlineStr" r="R21">
         <is>
-          <t xml:space="preserve">US78573M1045</t>
+          <t xml:space="preserve">SPYV440U</t>
         </is>
       </c>
       <c t="inlineStr" r="S21">
@@ -2238,26 +2235,21 @@
       <c t="inlineStr" r="V21">
         <is>
           <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="W21">
-        <is>
-          <t xml:space="preserve">SABR US Equity</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="65">
-        <v>49547</v>
+        <v>48370</v>
       </c>
       <c t="inlineStr" r="B22">
         <is>
-          <t xml:space="preserve">Kingsoft Cloud Holdings Ltd</t>
+          <t xml:space="preserve">Irhythm Technologies Inc.</t>
         </is>
       </c>
       <c t="inlineStr" r="C22">
         <is>
-          <t xml:space="preserve">KC US Equity</t>
+          <t xml:space="preserve">IRTC US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D22">
@@ -2267,7 +2259,7 @@
       </c>
       <c t="inlineStr" r="E22">
         <is>
-          <t xml:space="preserve">Information Technology</t>
+          <t xml:space="preserve">Health Care</t>
         </is>
       </c>
       <c t="inlineStr" r="F22">
@@ -2281,25 +2273,25 @@
         </is>
       </c>
       <c r="H22" s="63">
-        <v>52936</v>
+        <v>34924</v>
       </c>
       <c r="I22" s="63">
-        <v>2011122</v>
+        <v>2150423</v>
       </c>
       <c r="J22" s="56">
-        <v>0.031</v>
+        <v>0.032799999999999996</v>
       </c>
       <c r="K22" s="63">
-        <v>1914259</v>
+        <v>2338335</v>
       </c>
       <c r="L22" s="66">
-        <v>36.16</v>
+        <v>66.95</v>
       </c>
       <c r="M22" s="66">
-        <v>37.99</v>
+        <v>61.57</v>
       </c>
       <c r="N22" s="56">
-        <v>0.0506</v>
+        <v>-0.08039999999999999</v>
       </c>
       <c r="O22" s="56">
         <v>0</v>
@@ -2307,14 +2299,12 @@
       <c t="n" r="P22">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q22">
-        <is>
-          <t xml:space="preserve">49639K101</t>
-        </is>
+      <c r="Q22" s="65">
+        <v>450056106</v>
       </c>
       <c t="inlineStr" r="R22">
         <is>
-          <t xml:space="preserve">US49639K1016</t>
+          <t xml:space="preserve">US4500561067</t>
         </is>
       </c>
       <c t="inlineStr" r="S22">
@@ -2339,22 +2329,22 @@
       </c>
       <c t="inlineStr" r="W22">
         <is>
-          <t xml:space="preserve">KC US Equity</t>
+          <t xml:space="preserve">IRTC US Equity</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="65">
-        <v>49359</v>
+        <v>38802</v>
       </c>
       <c t="inlineStr" r="B23">
         <is>
-          <t xml:space="preserve">Yatsen Holding Ltd</t>
+          <t xml:space="preserve">Sabre Corporation</t>
         </is>
       </c>
       <c t="inlineStr" r="C23">
         <is>
-          <t xml:space="preserve">YSG US Equity</t>
+          <t xml:space="preserve">SABR US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D23">
@@ -2364,7 +2354,7 @@
       </c>
       <c t="inlineStr" r="E23">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Information Technology</t>
         </is>
       </c>
       <c t="inlineStr" r="F23">
@@ -2378,25 +2368,25 @@
         </is>
       </c>
       <c r="H23" s="63">
-        <v>272591</v>
+        <v>146057</v>
       </c>
       <c r="I23" s="63">
-        <v>2004640</v>
+        <v>2055204</v>
       </c>
       <c r="J23" s="56">
-        <v>0.030899999999999997</v>
+        <v>0.031400000000000004</v>
       </c>
       <c r="K23" s="63">
-        <v>2067052</v>
+        <v>2304989</v>
       </c>
       <c r="L23" s="66">
-        <v>7.58</v>
+        <v>15.78</v>
       </c>
       <c r="M23" s="66">
-        <v>7.35</v>
+        <v>14.07</v>
       </c>
       <c r="N23" s="56">
-        <v>-0.0302</v>
+        <v>-0.1084</v>
       </c>
       <c r="O23" s="56">
         <v>0</v>
@@ -2404,12 +2394,14 @@
       <c t="n" r="P23">
         <v>0</v>
       </c>
-      <c r="Q23" s="65">
-        <v>985194109</v>
+      <c t="inlineStr" r="Q23">
+        <is>
+          <t xml:space="preserve">78573M104</t>
+        </is>
       </c>
       <c t="inlineStr" r="R23">
         <is>
-          <t xml:space="preserve">US9851941099</t>
+          <t xml:space="preserve">US78573M1045</t>
         </is>
       </c>
       <c t="inlineStr" r="S23">
@@ -2434,32 +2426,32 @@
       </c>
       <c t="inlineStr" r="W23">
         <is>
-          <t xml:space="preserve">YSG US Equity</t>
+          <t xml:space="preserve">SABR US Equity</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="65">
-        <v>49005</v>
+        <v>40752</v>
       </c>
       <c t="inlineStr" r="B24">
         <is>
-          <t xml:space="preserve">Autohome Inc., Adr</t>
+          <t xml:space="preserve">Melia Hotels International, S.A.</t>
         </is>
       </c>
       <c t="inlineStr" r="C24">
         <is>
-          <t xml:space="preserve">ATHM US Equity</t>
+          <t xml:space="preserve">MEL SM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D24">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E24">
         <is>
-          <t xml:space="preserve">Communication Services</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F24">
@@ -2469,29 +2461,29 @@
       </c>
       <c t="inlineStr" r="G24">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
+          <t xml:space="preserve">Foreign Stock</t>
         </is>
       </c>
       <c r="H24" s="63">
-        <v>38396</v>
+        <v>204105</v>
       </c>
       <c r="I24" s="63">
-        <v>1944644</v>
+        <v>1786870</v>
       </c>
       <c r="J24" s="56">
-        <v>0.03</v>
+        <v>0.0273</v>
       </c>
       <c r="K24" s="63">
-        <v>2043278</v>
+        <v>1876695</v>
       </c>
       <c r="L24" s="66">
-        <v>53.22</v>
+        <v>9.19</v>
       </c>
       <c r="M24" s="66">
-        <v>50.65</v>
+        <v>8.75</v>
       </c>
       <c r="N24" s="56">
-        <v>-0.0483</v>
+        <v>-0.0479</v>
       </c>
       <c r="O24" s="56">
         <v>0</v>
@@ -2499,14 +2491,9 @@
       <c t="n" r="P24">
         <v>0</v>
       </c>
-      <c t="inlineStr" r="Q24">
-        <is>
-          <t xml:space="preserve">05278C107</t>
-        </is>
-      </c>
       <c t="inlineStr" r="R24">
         <is>
-          <t xml:space="preserve">US05278C1071</t>
+          <t xml:space="preserve">ES0176252718</t>
         </is>
       </c>
       <c t="inlineStr" r="S24">
@@ -2531,27 +2518,27 @@
       </c>
       <c t="inlineStr" r="W24">
         <is>
-          <t xml:space="preserve">ATHM US Equity</t>
+          <t xml:space="preserve">MEL SM Equity</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="65">
-        <v>40752</v>
+        <v>49359</v>
       </c>
       <c t="inlineStr" r="B25">
         <is>
-          <t xml:space="preserve">Melia Hotels International, S.A.</t>
+          <t xml:space="preserve">Yatsen Holding Ltd</t>
         </is>
       </c>
       <c t="inlineStr" r="C25">
         <is>
-          <t xml:space="preserve">MEL SM Equity</t>
+          <t xml:space="preserve">YSG US Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D25">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E25">
@@ -2566,29 +2553,29 @@
       </c>
       <c t="inlineStr" r="G25">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H25" s="63">
-        <v>204105</v>
+        <v>272591</v>
       </c>
       <c r="I25" s="63">
-        <v>1864764</v>
+        <v>1755728</v>
       </c>
       <c r="J25" s="56">
-        <v>0.0288</v>
+        <v>0.0268</v>
       </c>
       <c r="K25" s="63">
-        <v>1858737</v>
+        <v>2077147</v>
       </c>
       <c r="L25" s="66">
-        <v>9.11</v>
+        <v>7.62</v>
       </c>
       <c r="M25" s="66">
-        <v>9.14</v>
+        <v>6.44</v>
       </c>
       <c r="N25" s="56">
-        <v>0.0032</v>
+        <v>-0.1547</v>
       </c>
       <c r="O25" s="56">
         <v>0</v>
@@ -2596,9 +2583,12 @@
       <c t="n" r="P25">
         <v>0</v>
       </c>
+      <c r="Q25" s="65">
+        <v>985194109</v>
+      </c>
       <c t="inlineStr" r="R25">
         <is>
-          <t xml:space="preserve">ES0176252718</t>
+          <t xml:space="preserve">US9851941099</t>
         </is>
       </c>
       <c t="inlineStr" r="S25">
@@ -2623,7 +2613,7 @@
       </c>
       <c t="inlineStr" r="W25">
         <is>
-          <t xml:space="preserve">MEL SM Equity</t>
+          <t xml:space="preserve">YSG US Equity</t>
         </is>
       </c>
     </row>
@@ -2665,22 +2655,22 @@
         <v>688907</v>
       </c>
       <c r="I26" s="63">
-        <v>1790592</v>
+        <v>1749156</v>
       </c>
       <c r="J26" s="56">
-        <v>0.0276</v>
+        <v>0.026699999999999998</v>
       </c>
       <c r="K26" s="63">
-        <v>1717219</v>
+        <v>1735324</v>
       </c>
       <c r="L26" s="66">
-        <v>2.49</v>
+        <v>2.52</v>
       </c>
       <c r="M26" s="66">
-        <v>2.60</v>
+        <v>2.54</v>
       </c>
       <c r="N26" s="56">
-        <v>0.042699999999999995</v>
+        <v>0.008</v>
       </c>
       <c r="O26" s="56">
         <v>0</v>
@@ -2721,26 +2711,26 @@
     </row>
     <row r="27">
       <c r="A27" s="65">
-        <v>40753</v>
+        <v>47562</v>
       </c>
       <c t="inlineStr" r="B27">
         <is>
-          <t xml:space="preserve">Ssp Group Plc</t>
+          <t xml:space="preserve">Cielo Sa</t>
         </is>
       </c>
       <c t="inlineStr" r="C27">
         <is>
-          <t xml:space="preserve">SSPG LN Equity</t>
+          <t xml:space="preserve">CIEL3 BZ Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D27">
         <is>
-          <t xml:space="preserve">United Kingdom</t>
+          <t xml:space="preserve">Brazil</t>
         </is>
       </c>
       <c t="inlineStr" r="E27">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Information Technology</t>
         </is>
       </c>
       <c t="inlineStr" r="F27">
@@ -2750,39 +2740,44 @@
       </c>
       <c t="inlineStr" r="G27">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Domestic Stock</t>
         </is>
       </c>
       <c r="H27" s="63">
-        <v>369508</v>
+        <v>2881500</v>
       </c>
       <c r="I27" s="63">
-        <v>1758204</v>
+        <v>1737988</v>
       </c>
       <c r="J27" s="56">
-        <v>0.0271</v>
+        <v>0.0265</v>
       </c>
       <c r="K27" s="63">
-        <v>1910124</v>
+        <v>2789782</v>
       </c>
       <c r="L27" s="66">
-        <v>5.17</v>
+        <v>0.97</v>
       </c>
       <c r="M27" s="66">
-        <v>4.76</v>
+        <v>0.60</v>
       </c>
       <c r="N27" s="56">
-        <v>-0.0795</v>
+        <v>-0.377</v>
       </c>
       <c r="O27" s="56">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c t="n" r="P27">
         <v>0</v>
       </c>
+      <c t="inlineStr" r="Q27">
+        <is>
+          <t xml:space="preserve">P2859E100</t>
+        </is>
+      </c>
       <c t="inlineStr" r="R27">
         <is>
-          <t xml:space="preserve">GB00BGBN7C04</t>
+          <t xml:space="preserve">BRCIELACNOR3</t>
         </is>
       </c>
       <c t="inlineStr" r="S27">
@@ -2807,27 +2802,27 @@
       </c>
       <c t="inlineStr" r="W27">
         <is>
-          <t xml:space="preserve">SSPPF Equity</t>
+          <t xml:space="preserve">CIEL3 BZ Equity</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="65">
-        <v>38602</v>
+        <v>40753</v>
       </c>
       <c t="inlineStr" r="B28">
         <is>
-          <t xml:space="preserve">Autogrill S.P.A.</t>
+          <t xml:space="preserve">Ssp Group Plc</t>
         </is>
       </c>
       <c t="inlineStr" r="C28">
         <is>
-          <t xml:space="preserve">AGL IM Equity</t>
+          <t xml:space="preserve">SSPG LN Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D28">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United Kingdom</t>
         </is>
       </c>
       <c t="inlineStr" r="E28">
@@ -2846,25 +2841,25 @@
         </is>
       </c>
       <c r="H28" s="63">
-        <v>178577</v>
+        <v>369508</v>
       </c>
       <c r="I28" s="63">
-        <v>1725762</v>
+        <v>1666099</v>
       </c>
       <c r="J28" s="56">
-        <v>0.026600000000000002</v>
+        <v>0.0254</v>
       </c>
       <c r="K28" s="63">
-        <v>1457977</v>
+        <v>1930262</v>
       </c>
       <c r="L28" s="66">
-        <v>8.16</v>
+        <v>5.22</v>
       </c>
       <c r="M28" s="66">
-        <v>9.66</v>
+        <v>4.51</v>
       </c>
       <c r="N28" s="56">
-        <v>0.1837</v>
+        <v>-0.1369</v>
       </c>
       <c r="O28" s="56">
         <v>0</v>
@@ -2874,7 +2869,7 @@
       </c>
       <c t="inlineStr" r="R28">
         <is>
-          <t xml:space="preserve">IT0001137345</t>
+          <t xml:space="preserve">GB00BGBN7C04</t>
         </is>
       </c>
       <c t="inlineStr" r="S28">
@@ -2899,7 +2894,7 @@
       </c>
       <c t="inlineStr" r="W28">
         <is>
-          <t xml:space="preserve">AGL IM Equity</t>
+          <t xml:space="preserve">SSPPF Equity</t>
         </is>
       </c>
     </row>
@@ -2941,22 +2936,22 @@
         <v>569481</v>
       </c>
       <c r="I29" s="63">
-        <v>1455751</v>
+        <v>1621398</v>
       </c>
       <c r="J29" s="56">
-        <v>0.0225</v>
+        <v>0.0248</v>
       </c>
       <c r="K29" s="63">
-        <v>3276293</v>
+        <v>3291247</v>
       </c>
       <c r="L29" s="66">
-        <v>5.75</v>
+        <v>5.78</v>
       </c>
       <c r="M29" s="66">
-        <v>2.56</v>
+        <v>2.85</v>
       </c>
       <c r="N29" s="56">
-        <v>-0.5557</v>
+        <v>-0.5074000000000001</v>
       </c>
       <c r="O29" s="56">
         <v>-0.0002</v>
@@ -3000,21 +2995,21 @@
     </row>
     <row r="30">
       <c r="A30" s="65">
-        <v>48704</v>
+        <v>38602</v>
       </c>
       <c t="inlineStr" r="B30">
         <is>
-          <t xml:space="preserve">New Oriental Education &amp; Technology Group Inc</t>
+          <t xml:space="preserve">Autogrill S.P.A.</t>
         </is>
       </c>
       <c t="inlineStr" r="C30">
         <is>
-          <t xml:space="preserve">9901 HK Equity</t>
+          <t xml:space="preserve">AGL IM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D30">
         <is>
-          <t xml:space="preserve">Hong Kong</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E30">
@@ -3033,25 +3028,25 @@
         </is>
       </c>
       <c r="H30" s="63">
-        <v>509900</v>
+        <v>178577</v>
       </c>
       <c r="I30" s="63">
-        <v>1276875</v>
+        <v>1615761</v>
       </c>
       <c r="J30" s="56">
-        <v>0.0197</v>
+        <v>0.024700000000000003</v>
       </c>
       <c r="K30" s="63">
-        <v>1441329</v>
+        <v>1472063</v>
       </c>
       <c r="L30" s="66">
-        <v>2.83</v>
+        <v>8.24</v>
       </c>
       <c r="M30" s="66">
-        <v>2.50</v>
+        <v>9.05</v>
       </c>
       <c r="N30" s="56">
-        <v>-0.11410000000000001</v>
+        <v>0.09759999999999999</v>
       </c>
       <c r="O30" s="56">
         <v>0</v>
@@ -3059,12 +3054,9 @@
       <c t="n" r="P30">
         <v>0</v>
       </c>
-      <c r="Q30" s="65">
-        <v>0</v>
-      </c>
       <c t="inlineStr" r="R30">
         <is>
-          <t xml:space="preserve">KYG6470A1168</t>
+          <t xml:space="preserve">IT0001137345</t>
         </is>
       </c>
       <c t="inlineStr" r="S30">
@@ -3089,32 +3081,32 @@
       </c>
       <c t="inlineStr" r="W30">
         <is>
-          <t xml:space="preserve">9901 HK Equity</t>
+          <t xml:space="preserve">AGL IM Equity</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="65">
-        <v>8739</v>
+        <v>48704</v>
       </c>
       <c t="inlineStr" r="B31">
         <is>
-          <t xml:space="preserve">Aena Sa</t>
+          <t xml:space="preserve">New Oriental Education &amp; Technology Group Inc</t>
         </is>
       </c>
       <c t="inlineStr" r="C31">
         <is>
-          <t xml:space="preserve">AENA SM Equity</t>
+          <t xml:space="preserve">9901 HK Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D31">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">Hong Kong</t>
         </is>
       </c>
       <c t="inlineStr" r="E31">
         <is>
-          <t xml:space="preserve">Industrials</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F31">
@@ -3128,25 +3120,25 @@
         </is>
       </c>
       <c r="H31" s="63">
-        <v>6255</v>
+        <v>509900</v>
       </c>
       <c r="I31" s="63">
-        <v>1265052</v>
+        <v>1410234</v>
       </c>
       <c r="J31" s="56">
-        <v>0.0195</v>
+        <v>0.0215</v>
       </c>
       <c r="K31" s="63">
-        <v>1306650</v>
+        <v>1449533</v>
       </c>
       <c r="L31" s="66">
-        <v>208.90</v>
+        <v>2.84</v>
       </c>
       <c r="M31" s="66">
-        <v>202.25</v>
+        <v>2.77</v>
       </c>
       <c r="N31" s="56">
-        <v>-0.0318</v>
+        <v>-0.0271</v>
       </c>
       <c r="O31" s="56">
         <v>0</v>
@@ -3154,9 +3146,12 @@
       <c t="n" r="P31">
         <v>0</v>
       </c>
+      <c r="Q31" s="65">
+        <v>0</v>
+      </c>
       <c t="inlineStr" r="R31">
         <is>
-          <t xml:space="preserve">ES0105046009</t>
+          <t xml:space="preserve">KYG6470A1168</t>
         </is>
       </c>
       <c t="inlineStr" r="S31">
@@ -3181,22 +3176,22 @@
       </c>
       <c t="inlineStr" r="W31">
         <is>
-          <t xml:space="preserve">ES0105046009 Equity</t>
+          <t xml:space="preserve">9901 HK Equity</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="65">
-        <v>38605</v>
+        <v>8739</v>
       </c>
       <c t="inlineStr" r="B32">
         <is>
-          <t xml:space="preserve">Mtu Aero Engines Ag</t>
+          <t xml:space="preserve">Aena Sa</t>
         </is>
       </c>
       <c t="inlineStr" r="C32">
         <is>
-          <t xml:space="preserve">MTX GR Equity</t>
+          <t xml:space="preserve">AENA SM Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D32">
@@ -3220,25 +3215,25 @@
         </is>
       </c>
       <c r="H32" s="63">
-        <v>4247</v>
+        <v>6255</v>
       </c>
       <c r="I32" s="63">
-        <v>1245449</v>
+        <v>1245448</v>
       </c>
       <c r="J32" s="56">
-        <v>0.0192</v>
+        <v>0.019</v>
       </c>
       <c r="K32" s="63">
-        <v>1250305</v>
+        <v>1319274</v>
       </c>
       <c r="L32" s="66">
-        <v>294.40</v>
+        <v>210.92</v>
       </c>
       <c r="M32" s="66">
-        <v>293.25</v>
+        <v>199.11</v>
       </c>
       <c r="N32" s="56">
-        <v>-0.0039000000000000003</v>
+        <v>-0.055999999999999994</v>
       </c>
       <c r="O32" s="56">
         <v>0</v>
@@ -3248,7 +3243,7 @@
       </c>
       <c t="inlineStr" r="R32">
         <is>
-          <t xml:space="preserve">DE000A0D9PT0</t>
+          <t xml:space="preserve">ES0105046009</t>
         </is>
       </c>
       <c t="inlineStr" r="S32">
@@ -3273,64 +3268,64 @@
       </c>
       <c t="inlineStr" r="W32">
         <is>
-          <t xml:space="preserve">MTX GR Equity</t>
+          <t xml:space="preserve">ES0105046009 Equity</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="65">
-        <v>49548</v>
+        <v>38605</v>
       </c>
       <c t="inlineStr" r="B33">
         <is>
-          <t xml:space="preserve">Alibaba Group Holding Lt Call 180 12/17/21</t>
+          <t xml:space="preserve">Mtu Aero Engines Ag</t>
         </is>
       </c>
       <c t="inlineStr" r="C33">
         <is>
-          <t xml:space="preserve">BABA US 12/17/21 C180 Equity</t>
+          <t xml:space="preserve">MTX GR Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D33">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E33">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Industrials</t>
         </is>
       </c>
       <c t="inlineStr" r="F33">
         <is>
-          <t xml:space="preserve">Option</t>
+          <t xml:space="preserve">Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="G33">
         <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c r="H33" s="65">
-        <v>500</v>
+          <t xml:space="preserve">Foreign Stock</t>
+        </is>
+      </c>
+      <c r="H33" s="63">
+        <v>4247</v>
       </c>
       <c r="I33" s="63">
-        <v>720921</v>
+        <v>1206000</v>
       </c>
       <c r="J33" s="56">
-        <v>0.0111</v>
+        <v>0.0184</v>
       </c>
       <c r="K33" s="63">
-        <v>845744</v>
+        <v>1262385</v>
       </c>
       <c r="L33" s="66">
-        <v>16.91</v>
+        <v>297.24</v>
       </c>
       <c r="M33" s="66">
-        <v>14.42</v>
+        <v>283.97</v>
       </c>
       <c r="N33" s="56">
-        <v>-0.1476</v>
+        <v>-0.0447</v>
       </c>
       <c r="O33" s="56">
         <v>0</v>
@@ -3340,7 +3335,7 @@
       </c>
       <c t="inlineStr" r="R33">
         <is>
-          <t xml:space="preserve">BABAL180U</t>
+          <t xml:space="preserve">DE000A0D9PT0</t>
         </is>
       </c>
       <c t="inlineStr" r="S33">
@@ -3361,21 +3356,26 @@
       <c t="inlineStr" r="V33">
         <is>
           <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="W33">
+        <is>
+          <t xml:space="preserve">MTX GR Equity</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="65">
-        <v>48199</v>
+        <v>49549</v>
       </c>
       <c t="inlineStr" r="B34">
         <is>
-          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 430 09/17/21</t>
+          <t xml:space="preserve">Baidu Inc Call 170 12/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C34">
         <is>
-          <t xml:space="preserve">SPY US 09/17/21 P430 Equity</t>
+          <t xml:space="preserve">BIDU US 12/17/21 C170 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D34">
@@ -3385,7 +3385,7 @@
       </c>
       <c t="inlineStr" r="E34">
         <is>
-          <t xml:space="preserve">Equity Index</t>
+          <t xml:space="preserve">Communication Services</t>
         </is>
       </c>
       <c t="inlineStr" r="F34">
@@ -3398,36 +3398,36 @@
           <t xml:space="preserve">Option</t>
         </is>
       </c>
-      <c r="H34" s="63">
-        <v>3000</v>
+      <c r="H34" s="65">
+        <v>400</v>
       </c>
       <c r="I34" s="63">
-        <v>710217</v>
+        <v>569430</v>
       </c>
       <c r="J34" s="56">
-        <v>0.011000000000000001</v>
+        <v>0.0087</v>
       </c>
       <c r="K34" s="63">
-        <v>2297892</v>
+        <v>390882</v>
       </c>
       <c r="L34" s="66">
-        <v>7.66</v>
+        <v>9.77</v>
       </c>
       <c r="M34" s="66">
-        <v>2.37</v>
+        <v>14.24</v>
       </c>
       <c r="N34" s="56">
-        <v>-0.6909000000000001</v>
+        <v>0.4568</v>
       </c>
       <c r="O34" s="56">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c t="n" r="P34">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R34">
         <is>
-          <t xml:space="preserve">SPYU430U</t>
+          <t xml:space="preserve">BIDUL170U</t>
         </is>
       </c>
       <c t="inlineStr" r="S34">
@@ -3453,16 +3453,16 @@
     </row>
     <row r="35">
       <c r="A35" s="65">
-        <v>49549</v>
+        <v>49548</v>
       </c>
       <c t="inlineStr" r="B35">
         <is>
-          <t xml:space="preserve">Baidu Inc Call 170 12/17/21</t>
+          <t xml:space="preserve">Alibaba Group Holding Lt Call 180 12/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C35">
         <is>
-          <t xml:space="preserve">BIDU US 12/17/21 C170 Equity</t>
+          <t xml:space="preserve">BABA US 12/17/21 C180 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D35">
@@ -3472,7 +3472,7 @@
       </c>
       <c t="inlineStr" r="E35">
         <is>
-          <t xml:space="preserve">Communication Services</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F35">
@@ -3486,25 +3486,25 @@
         </is>
       </c>
       <c r="H35" s="65">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="I35" s="63">
-        <v>400442</v>
+        <v>566267</v>
       </c>
       <c r="J35" s="56">
-        <v>0.0062</v>
+        <v>0.0086</v>
       </c>
       <c r="K35" s="63">
-        <v>388982</v>
+        <v>849874</v>
       </c>
       <c r="L35" s="66">
-        <v>9.72</v>
+        <v>17.00</v>
       </c>
       <c r="M35" s="66">
-        <v>10.01</v>
+        <v>11.33</v>
       </c>
       <c r="N35" s="56">
-        <v>0.029500000000000002</v>
+        <v>-0.3337</v>
       </c>
       <c r="O35" s="56">
         <v>0</v>
@@ -3514,7 +3514,7 @@
       </c>
       <c t="inlineStr" r="R35">
         <is>
-          <t xml:space="preserve">BIDUL170U</t>
+          <t xml:space="preserve">BABAL180U</t>
         </is>
       </c>
       <c t="inlineStr" r="S35">
@@ -3540,68 +3540,68 @@
     </row>
     <row r="36">
       <c r="A36" s="65">
-        <v>38603</v>
+        <v>48199</v>
       </c>
       <c t="inlineStr" r="B36">
         <is>
-          <t xml:space="preserve">Krones AG</t>
+          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 430 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C36">
         <is>
-          <t xml:space="preserve">KRN GR Equity</t>
+          <t xml:space="preserve">SPY US 09/17/21 P430 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D36">
         <is>
-          <t xml:space="preserve">Europe</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E36">
         <is>
-          <t xml:space="preserve">Industrials</t>
+          <t xml:space="preserve">Equity Index</t>
         </is>
       </c>
       <c t="inlineStr" r="F36">
         <is>
-          <t xml:space="preserve">Equity</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c t="inlineStr" r="G36">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c r="H36" s="63">
-        <v>1081</v>
+        <v>3000</v>
       </c>
       <c r="I36" s="63">
-        <v>137234</v>
+        <v>280919</v>
       </c>
       <c r="J36" s="56">
-        <v>0.0021</v>
+        <v>0.0043</v>
       </c>
       <c r="K36" s="63">
-        <v>94570</v>
+        <v>2309115</v>
       </c>
       <c r="L36" s="66">
-        <v>87.48</v>
+        <v>7.70</v>
       </c>
       <c r="M36" s="66">
-        <v>126.95</v>
+        <v>0.94</v>
       </c>
       <c r="N36" s="56">
-        <v>0.4511</v>
+        <v>-0.8783</v>
       </c>
       <c r="O36" s="56">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c t="n" r="P36">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R36">
         <is>
-          <t xml:space="preserve">DE0006335003</t>
+          <t xml:space="preserve">SPYU430U</t>
         </is>
       </c>
       <c t="inlineStr" r="S36">
@@ -3622,68 +3622,63 @@
       <c t="inlineStr" r="V36">
         <is>
           <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="W36">
-        <is>
-          <t xml:space="preserve">KRN GR Equity</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="65">
-        <v>49007</v>
+        <v>38603</v>
       </c>
       <c t="inlineStr" r="B37">
         <is>
-          <t xml:space="preserve">Ke Holdings Inc Put 15 10/15/21</t>
+          <t xml:space="preserve">Krones AG</t>
         </is>
       </c>
       <c t="inlineStr" r="C37">
         <is>
-          <t xml:space="preserve">BEKE US 10/15/21 P15 Equity</t>
+          <t xml:space="preserve">KRN GR Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D37">
         <is>
-          <t xml:space="preserve">United States</t>
+          <t xml:space="preserve">Europe</t>
         </is>
       </c>
       <c t="inlineStr" r="E37">
         <is>
-          <t xml:space="preserve">Real Estate</t>
+          <t xml:space="preserve">Industrials</t>
         </is>
       </c>
       <c t="inlineStr" r="F37">
         <is>
-          <t xml:space="preserve">Option</t>
+          <t xml:space="preserve">Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="G37">
         <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c r="H37" s="65">
-        <v>750</v>
+          <t xml:space="preserve">Foreign Stock</t>
+        </is>
+      </c>
+      <c r="H37" s="63">
+        <v>1081</v>
       </c>
       <c r="I37" s="63">
-        <v>104833</v>
+        <v>144545</v>
       </c>
       <c r="J37" s="56">
-        <v>0.0016</v>
+        <v>0.0022</v>
       </c>
       <c r="K37" s="63">
-        <v>129388</v>
+        <v>95484</v>
       </c>
       <c r="L37" s="66">
-        <v>1.73</v>
+        <v>88.33</v>
       </c>
       <c r="M37" s="66">
-        <v>1.40</v>
+        <v>133.71</v>
       </c>
       <c r="N37" s="56">
-        <v>-0.1898</v>
+        <v>0.5138</v>
       </c>
       <c r="O37" s="56">
         <v>0</v>
@@ -3693,7 +3688,7 @@
       </c>
       <c t="inlineStr" r="R37">
         <is>
-          <t xml:space="preserve">BEKEV15U</t>
+          <t xml:space="preserve">DE0006335003</t>
         </is>
       </c>
       <c t="inlineStr" r="S37">
@@ -3714,6 +3709,11 @@
       <c t="inlineStr" r="V37">
         <is>
           <t xml:space="preserve">-</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="W37">
+        <is>
+          <t xml:space="preserve">KRN GR Equity</t>
         </is>
       </c>
     </row>
@@ -3755,13 +3755,13 @@
         <v>440000</v>
       </c>
       <c r="I38" s="63">
-        <v>72601</v>
+        <v>75878</v>
       </c>
       <c r="J38" s="56">
-        <v>0.0011</v>
+        <v>0.0012</v>
       </c>
       <c r="K38" s="63">
-        <v>83971</v>
+        <v>84449</v>
       </c>
       <c r="L38" s="66">
         <v>0.19</v>
@@ -3770,7 +3770,7 @@
         <v>0.17</v>
       </c>
       <c r="N38" s="56">
-        <v>-0.1354</v>
+        <v>-0.1015</v>
       </c>
       <c r="O38" s="56">
         <v>0</v>
@@ -3816,16 +3816,16 @@
     </row>
     <row r="39">
       <c r="A39" s="65">
-        <v>49009</v>
+        <v>49007</v>
       </c>
       <c t="inlineStr" r="B39">
         <is>
-          <t xml:space="preserve">Wynn Resorts Ltd Put 70 03/18/22</t>
+          <t xml:space="preserve">Ke Holdings Inc Put 15 10/15/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C39">
         <is>
-          <t xml:space="preserve">WYNN US 03/18/22 P70 Equity</t>
+          <t xml:space="preserve">BEKE US 10/15/21 P15 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D39">
@@ -3835,7 +3835,7 @@
       </c>
       <c t="inlineStr" r="E39">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Real Estate</t>
         </is>
       </c>
       <c t="inlineStr" r="F39">
@@ -3849,25 +3849,25 @@
         </is>
       </c>
       <c r="H39" s="65">
-        <v>200</v>
+        <v>750</v>
       </c>
       <c r="I39" s="63">
-        <v>69259</v>
+        <v>57892</v>
       </c>
       <c r="J39" s="56">
-        <v>0.0011</v>
+        <v>0.0009</v>
       </c>
       <c r="K39" s="63">
-        <v>89650</v>
+        <v>130020</v>
       </c>
       <c r="L39" s="66">
-        <v>4.48</v>
+        <v>1.73</v>
       </c>
       <c r="M39" s="66">
-        <v>3.46</v>
+        <v>0.77</v>
       </c>
       <c r="N39" s="56">
-        <v>-0.2275</v>
+        <v>-0.5547</v>
       </c>
       <c r="O39" s="56">
         <v>0</v>
@@ -3877,7 +3877,7 @@
       </c>
       <c t="inlineStr" r="R39">
         <is>
-          <t xml:space="preserve">WYNNO70U</t>
+          <t xml:space="preserve">BEKEV15U</t>
         </is>
       </c>
       <c t="inlineStr" r="S39">
@@ -3903,21 +3903,21 @@
     </row>
     <row r="40">
       <c r="A40" s="65">
-        <v>48371</v>
+        <v>49009</v>
       </c>
       <c t="inlineStr" r="B40">
         <is>
-          <t xml:space="preserve">Cineworld Group Plc</t>
+          <t xml:space="preserve">Wynn Resorts Ltd Put 70 03/18/22</t>
         </is>
       </c>
       <c t="inlineStr" r="C40">
         <is>
-          <t xml:space="preserve">CINE LN Equity</t>
+          <t xml:space="preserve">WYNN US 03/18/22 P70 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D40">
         <is>
-          <t xml:space="preserve">United Kingdom</t>
+          <t xml:space="preserve">United States</t>
         </is>
       </c>
       <c t="inlineStr" r="E40">
@@ -3927,34 +3927,34 @@
       </c>
       <c t="inlineStr" r="F40">
         <is>
-          <t xml:space="preserve">Equity</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c t="inlineStr" r="G40">
         <is>
-          <t xml:space="preserve">Foreign Stock</t>
-        </is>
-      </c>
-      <c r="H40" s="63">
-        <v>55150</v>
+          <t xml:space="preserve">Option</t>
+        </is>
+      </c>
+      <c r="H40" s="65">
+        <v>200</v>
       </c>
       <c r="I40" s="63">
-        <v>64486</v>
+        <v>52641</v>
       </c>
       <c r="J40" s="56">
-        <v>0.001</v>
+        <v>0.0008</v>
       </c>
       <c r="K40" s="63">
-        <v>58639</v>
+        <v>90088</v>
       </c>
       <c r="L40" s="66">
-        <v>1.06</v>
+        <v>4.50</v>
       </c>
       <c r="M40" s="66">
-        <v>1.17</v>
+        <v>2.63</v>
       </c>
       <c r="N40" s="56">
-        <v>0.09970000000000001</v>
+        <v>-0.4157</v>
       </c>
       <c r="O40" s="56">
         <v>0</v>
@@ -3964,7 +3964,7 @@
       </c>
       <c t="inlineStr" r="R40">
         <is>
-          <t xml:space="preserve">GB00B15FWH70</t>
+          <t xml:space="preserve">WYNNO70U</t>
         </is>
       </c>
       <c t="inlineStr" r="S40">
@@ -3985,26 +3985,21 @@
       <c t="inlineStr" r="V40">
         <is>
           <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="W40">
-        <is>
-          <t xml:space="preserve">CINE LN Equity</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="65">
-        <v>48873</v>
+        <v>47845</v>
       </c>
       <c t="inlineStr" r="B41">
         <is>
-          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 425 09/07/21</t>
+          <t xml:space="preserve">Tal Education Group Call 32.5 11/19/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C41">
         <is>
-          <t xml:space="preserve">SPY US 09/07/21 P425 Equity</t>
+          <t xml:space="preserve">TAL US 11/19/21 C32.5 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D41">
@@ -4014,7 +4009,7 @@
       </c>
       <c t="inlineStr" r="E41">
         <is>
-          <t xml:space="preserve">Equity Index</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F41">
@@ -4028,35 +4023,35 @@
         </is>
       </c>
       <c r="H41" s="63">
-        <v>1000</v>
+        <v>5100</v>
       </c>
       <c r="I41" s="63">
-        <v>54148</v>
+        <v>32268</v>
       </c>
       <c r="J41" s="56">
-        <v>0.0008</v>
+        <v>0.0005</v>
       </c>
       <c r="K41" s="63">
-        <v>598459</v>
+        <v>1280623</v>
       </c>
       <c r="L41" s="66">
-        <v>5.98</v>
+        <v>2.51</v>
       </c>
       <c r="M41" s="66">
-        <v>0.54</v>
+        <v>0.06</v>
       </c>
       <c r="N41" s="56">
-        <v>-0.9095</v>
+        <v>-0.9748</v>
       </c>
       <c r="O41" s="56">
-        <v>-0.0001</v>
+        <v>-0.0002</v>
       </c>
       <c t="n" r="P41">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R41">
         <is>
-          <t xml:space="preserve">SPY2U425U</t>
+          <t xml:space="preserve">TALK325U</t>
         </is>
       </c>
       <c t="inlineStr" r="S41">
@@ -4082,16 +4077,16 @@
     </row>
     <row r="42">
       <c r="A42" s="65">
-        <v>47845</v>
+        <v>47844</v>
       </c>
       <c t="inlineStr" r="B42">
         <is>
-          <t xml:space="preserve">Tal Education Group Call 32.5 11/19/21</t>
+          <t xml:space="preserve">Alibaba Group Holding Lt Call 230 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C42">
         <is>
-          <t xml:space="preserve">TAL US 11/19/21 C32.5 Equity</t>
+          <t xml:space="preserve">BABA US 09/17/21 C230 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D42">
@@ -4114,36 +4109,36 @@
           <t xml:space="preserve">Option</t>
         </is>
       </c>
-      <c r="H42" s="63">
-        <v>5100</v>
-      </c>
-      <c r="I42" s="63">
-        <v>19267</v>
-      </c>
-      <c r="J42" s="56">
-        <v>0.0003</v>
+      <c r="H42" s="65">
+        <v>280</v>
+      </c>
+      <c r="I42" s="65">
+        <v>709</v>
+      </c>
+      <c t="n" r="J42">
+        <v>0</v>
       </c>
       <c r="K42" s="63">
-        <v>1274399</v>
+        <v>232777</v>
       </c>
       <c r="L42" s="66">
-        <v>2.50</v>
+        <v>8.31</v>
       </c>
       <c r="M42" s="66">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="N42" s="56">
-        <v>-0.9849</v>
+        <v>-0.997</v>
       </c>
       <c r="O42" s="56">
-        <v>-0.0002</v>
+        <v>0</v>
       </c>
       <c t="n" r="P42">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R42">
         <is>
-          <t xml:space="preserve">TALK325U</t>
+          <t xml:space="preserve">BABAI230U</t>
         </is>
       </c>
       <c t="inlineStr" r="S42">
@@ -4169,16 +4164,16 @@
     </row>
     <row r="43">
       <c r="A43" s="65">
-        <v>47844</v>
+        <v>47901</v>
       </c>
       <c t="inlineStr" r="B43">
         <is>
-          <t xml:space="preserve">Alibaba Group Holding Lt Call 230 09/17/21</t>
+          <t xml:space="preserve">Alibaba Group Holding Lt Call 225 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C43">
         <is>
-          <t xml:space="preserve">BABA US 09/17/21 C230 Equity</t>
+          <t xml:space="preserve">BABA US 09/17/21 C225 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D43">
@@ -4202,25 +4197,25 @@
         </is>
       </c>
       <c r="H43" s="65">
-        <v>280</v>
-      </c>
-      <c r="I43" s="63">
-        <v>4936</v>
-      </c>
-      <c r="J43" s="56">
-        <v>0.0001</v>
+        <v>-140</v>
+      </c>
+      <c r="I43" s="65">
+        <v>-177</v>
+      </c>
+      <c t="n" r="J43">
+        <v>0</v>
       </c>
       <c r="K43" s="63">
-        <v>231645</v>
+        <v>-229903</v>
       </c>
       <c r="L43" s="66">
-        <v>8.27</v>
+        <v>16.42</v>
       </c>
       <c r="M43" s="66">
-        <v>0.18</v>
+        <v>0.01</v>
       </c>
       <c r="N43" s="56">
-        <v>-0.9787</v>
+        <v>-0.9992</v>
       </c>
       <c r="O43" s="56">
         <v>0</v>
@@ -4230,7 +4225,7 @@
       </c>
       <c t="inlineStr" r="R43">
         <is>
-          <t xml:space="preserve">BABAI230U</t>
+          <t xml:space="preserve">BABAI225U</t>
         </is>
       </c>
       <c t="inlineStr" r="S43">
@@ -4256,16 +4251,16 @@
     </row>
     <row r="44">
       <c r="A44" s="65">
-        <v>9331</v>
+        <v>49008</v>
       </c>
       <c t="inlineStr" r="B44">
         <is>
-          <t xml:space="preserve">Nokia Oyj, Sponsored Adr</t>
+          <t xml:space="preserve">Wynn Resorts Ltd Put 50 03/18/22</t>
         </is>
       </c>
       <c t="inlineStr" r="C44">
         <is>
-          <t xml:space="preserve">NOK US Equity</t>
+          <t xml:space="preserve">WYNN US 03/18/22 P50 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D44">
@@ -4275,62 +4270,49 @@
       </c>
       <c t="inlineStr" r="E44">
         <is>
-          <t xml:space="preserve">Information Technology</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F44">
         <is>
-          <t xml:space="preserve">Equity</t>
+          <t xml:space="preserve">Option</t>
         </is>
       </c>
       <c t="inlineStr" r="G44">
         <is>
-          <t xml:space="preserve">Domestic Stock</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H44">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="I44">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="n" r="J44">
-        <v>0</v>
-      </c>
-      <c t="inlineStr" r="K44">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="L44">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="M44">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="n" r="N44">
-        <v>0</v>
-      </c>
-      <c t="n" r="O44">
+          <t xml:space="preserve">Option</t>
+        </is>
+      </c>
+      <c r="H44" s="65">
+        <v>-200</v>
+      </c>
+      <c r="I44" s="63">
+        <v>-17083</v>
+      </c>
+      <c r="J44" s="56">
+        <v>-0.0003</v>
+      </c>
+      <c r="K44" s="63">
+        <v>-21008</v>
+      </c>
+      <c r="L44" s="66">
+        <v>1.05</v>
+      </c>
+      <c r="M44" s="66">
+        <v>0.85</v>
+      </c>
+      <c r="N44" s="56">
+        <v>-0.1868</v>
+      </c>
+      <c r="O44" s="56">
         <v>0</v>
       </c>
       <c t="n" r="P44">
         <v>0</v>
       </c>
-      <c r="Q44" s="65">
-        <v>654902204</v>
-      </c>
       <c t="inlineStr" r="R44">
         <is>
-          <t xml:space="preserve">US6549022043</t>
+          <t xml:space="preserve">WYNNO50U</t>
         </is>
       </c>
       <c t="inlineStr" r="S44">
@@ -4351,26 +4333,21 @@
       <c t="inlineStr" r="V44">
         <is>
           <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="W44">
-        <is>
-          <t xml:space="preserve">2640891 US Equity</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="65">
-        <v>47901</v>
+        <v>47304</v>
       </c>
       <c t="inlineStr" r="B45">
         <is>
-          <t xml:space="preserve">Alibaba Group Holding Lt Call 225 09/17/21</t>
+          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 410 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C45">
         <is>
-          <t xml:space="preserve">BABA US 09/17/21 C225 Equity</t>
+          <t xml:space="preserve">SPY US 09/17/21 P410 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D45">
@@ -4380,7 +4357,7 @@
       </c>
       <c t="inlineStr" r="E45">
         <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
+          <t xml:space="preserve">Equity Index</t>
         </is>
       </c>
       <c t="inlineStr" r="F45">
@@ -4393,36 +4370,36 @@
           <t xml:space="preserve">Option</t>
         </is>
       </c>
-      <c r="H45" s="65">
-        <v>-140</v>
+      <c r="H45" s="63">
+        <v>-3000</v>
       </c>
       <c r="I45" s="63">
-        <v>-2997</v>
-      </c>
-      <c t="n" r="J45">
-        <v>0</v>
+        <v>-102497</v>
+      </c>
+      <c r="J45" s="56">
+        <v>-0.0016</v>
       </c>
       <c r="K45" s="63">
-        <v>-228786</v>
+        <v>-1206970</v>
       </c>
       <c r="L45" s="66">
-        <v>16.34</v>
+        <v>4.02</v>
       </c>
       <c r="M45" s="66">
-        <v>0.21</v>
+        <v>0.34</v>
       </c>
       <c r="N45" s="56">
-        <v>-0.9869</v>
+        <v>-0.9151</v>
       </c>
       <c r="O45" s="56">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c t="n" r="P45">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R45">
         <is>
-          <t xml:space="preserve">BABAI225U</t>
+          <t xml:space="preserve">SPYU410U</t>
         </is>
       </c>
       <c t="inlineStr" r="S45">
@@ -4448,16 +4425,16 @@
     </row>
     <row r="46">
       <c r="A46" s="65">
-        <v>48872</v>
+        <v>49847</v>
       </c>
       <c t="inlineStr" r="B46">
         <is>
-          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 400 09/07/21</t>
+          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 420 10/15/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C46">
         <is>
-          <t xml:space="preserve">SPY US 09/07/21 P400 Equity</t>
+          <t xml:space="preserve">SPY US 10/15/21 P420 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D46">
@@ -4481,25 +4458,25 @@
         </is>
       </c>
       <c r="H46" s="63">
-        <v>-1000</v>
+        <v>-3000</v>
       </c>
       <c r="I46" s="63">
-        <v>-18889</v>
+        <v>-1089509</v>
       </c>
       <c r="J46" s="56">
-        <v>-0.0003</v>
+        <v>-0.0166</v>
       </c>
       <c r="K46" s="63">
-        <v>-239634</v>
+        <v>-1049057</v>
       </c>
       <c r="L46" s="66">
-        <v>2.40</v>
+        <v>3.50</v>
       </c>
       <c r="M46" s="66">
-        <v>0.19</v>
+        <v>3.63</v>
       </c>
       <c r="N46" s="56">
-        <v>-0.9212</v>
+        <v>0.038599999999999995</v>
       </c>
       <c r="O46" s="56">
         <v>0</v>
@@ -4509,7 +4486,7 @@
       </c>
       <c t="inlineStr" r="R46">
         <is>
-          <t xml:space="preserve">SPY2U400U</t>
+          <t xml:space="preserve">SPYV420U</t>
         </is>
       </c>
       <c t="inlineStr" r="S46">
@@ -4535,16 +4512,16 @@
     </row>
     <row r="47">
       <c r="A47" s="65">
-        <v>49008</v>
+        <v>48788</v>
       </c>
       <c t="inlineStr" r="B47">
         <is>
-          <t xml:space="preserve">Wynn Resorts Ltd Put 50 03/18/22</t>
+          <t xml:space="preserve">Tal Education Group Put 7.5 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C47">
         <is>
-          <t xml:space="preserve">WYNN US 03/18/22 P50 Equity</t>
+          <t xml:space="preserve">TAL US 09/17/21 P7.5 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D47">
@@ -4567,28 +4544,28 @@
           <t xml:space="preserve">Option</t>
         </is>
       </c>
-      <c r="H47" s="65">
-        <v>-200</v>
+      <c r="H47" s="63">
+        <v>-4000</v>
       </c>
       <c r="I47" s="63">
-        <v>-20526</v>
+        <v>-1113552</v>
       </c>
       <c r="J47" s="56">
-        <v>-0.0003</v>
+        <v>-0.017</v>
       </c>
       <c r="K47" s="63">
-        <v>-20906</v>
+        <v>-1229962</v>
       </c>
       <c r="L47" s="66">
-        <v>1.05</v>
+        <v>3.07</v>
       </c>
       <c r="M47" s="66">
-        <v>1.03</v>
+        <v>2.78</v>
       </c>
       <c r="N47" s="56">
-        <v>-0.0182</v>
-      </c>
-      <c t="n" r="O47">
+        <v>-0.0946</v>
+      </c>
+      <c r="O47" s="56">
         <v>0</v>
       </c>
       <c t="n" r="P47">
@@ -4596,7 +4573,7 @@
       </c>
       <c t="inlineStr" r="R47">
         <is>
-          <t xml:space="preserve">WYNNO50U</t>
+          <t xml:space="preserve">TALU75U</t>
         </is>
       </c>
       <c t="inlineStr" r="S47">
@@ -4622,16 +4599,16 @@
     </row>
     <row r="48">
       <c r="A48" s="65">
-        <v>47304</v>
+        <v>48787</v>
       </c>
       <c t="inlineStr" r="B48">
         <is>
-          <t xml:space="preserve">Spdr S&amp;P 500 ETF Trust Put 410 09/17/21</t>
+          <t xml:space="preserve">New Oriental Education &amp; T Put 4.5 09/17/21</t>
         </is>
       </c>
       <c t="inlineStr" r="C48">
         <is>
-          <t xml:space="preserve">SPY US 09/17/21 P410 Equity</t>
+          <t xml:space="preserve">EDU US 09/17/21 P4.5 Equity</t>
         </is>
       </c>
       <c t="inlineStr" r="D48">
@@ -4641,7 +4618,7 @@
       </c>
       <c t="inlineStr" r="E48">
         <is>
-          <t xml:space="preserve">Equity Index</t>
+          <t xml:space="preserve">Consumer Discretionary</t>
         </is>
       </c>
       <c t="inlineStr" r="F48">
@@ -4655,35 +4632,35 @@
         </is>
       </c>
       <c r="H48" s="63">
-        <v>-3000</v>
+        <v>-4311</v>
       </c>
       <c r="I48" s="63">
-        <v>-313553</v>
+        <v>-1227406</v>
       </c>
       <c r="J48" s="56">
-        <v>-0.0048</v>
+        <v>-0.0187</v>
       </c>
       <c r="K48" s="63">
-        <v>-1201104</v>
+        <v>-1243765</v>
       </c>
       <c r="L48" s="66">
-        <v>4.00</v>
+        <v>2.89</v>
       </c>
       <c r="M48" s="66">
-        <v>1.05</v>
+        <v>2.85</v>
       </c>
       <c r="N48" s="56">
-        <v>-0.7389</v>
+        <v>-0.0132</v>
       </c>
       <c r="O48" s="56">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c t="n" r="P48">
         <v>0</v>
       </c>
       <c t="inlineStr" r="R48">
         <is>
-          <t xml:space="preserve">SPYU410U</t>
+          <t xml:space="preserve">EDUU45U</t>
         </is>
       </c>
       <c t="inlineStr" r="S48">
@@ -4702,180 +4679,6 @@
         </is>
       </c>
       <c t="inlineStr" r="V48">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="65">
-        <v>48788</v>
-      </c>
-      <c t="inlineStr" r="B49">
-        <is>
-          <t xml:space="preserve">Tal Education Group Put 7.5 09/17/21</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C49">
-        <is>
-          <t xml:space="preserve">TAL US 09/17/21 P7.5 Equity</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D49">
-        <is>
-          <t xml:space="preserve">United States</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="E49">
-        <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F49">
-        <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G49">
-        <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c r="H49" s="63">
-        <v>-4000</v>
-      </c>
-      <c r="I49" s="63">
-        <v>-1324731</v>
-      </c>
-      <c r="J49" s="56">
-        <v>-0.0204</v>
-      </c>
-      <c r="K49" s="63">
-        <v>-1223985</v>
-      </c>
-      <c r="L49" s="66">
-        <v>3.06</v>
-      </c>
-      <c r="M49" s="66">
-        <v>3.31</v>
-      </c>
-      <c r="N49" s="56">
-        <v>0.0823</v>
-      </c>
-      <c r="O49" s="56">
-        <v>0</v>
-      </c>
-      <c t="n" r="P49">
-        <v>0</v>
-      </c>
-      <c t="inlineStr" r="R49">
-        <is>
-          <t xml:space="preserve">TALU75U</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="S49">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="T49">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="U49">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="V49">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="65">
-        <v>48787</v>
-      </c>
-      <c t="inlineStr" r="B50">
-        <is>
-          <t xml:space="preserve">New Oriental Education &amp; T Put 4.5 09/17/21</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C50">
-        <is>
-          <t xml:space="preserve">EDU US 09/17/21 P4.5 Equity</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="D50">
-        <is>
-          <t xml:space="preserve">United States</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="E50">
-        <is>
-          <t xml:space="preserve">Consumer Discretionary</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F50">
-        <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G50">
-        <is>
-          <t xml:space="preserve">Option</t>
-        </is>
-      </c>
-      <c r="H50" s="63">
-        <v>-4311</v>
-      </c>
-      <c r="I50" s="63">
-        <v>-1357157</v>
-      </c>
-      <c r="J50" s="56">
-        <v>-0.0209</v>
-      </c>
-      <c r="K50" s="63">
-        <v>-1237720</v>
-      </c>
-      <c r="L50" s="66">
-        <v>2.87</v>
-      </c>
-      <c r="M50" s="66">
-        <v>3.15</v>
-      </c>
-      <c r="N50" s="56">
-        <v>0.0965</v>
-      </c>
-      <c r="O50" s="56">
-        <v>0</v>
-      </c>
-      <c t="n" r="P50">
-        <v>0</v>
-      </c>
-      <c t="inlineStr" r="R50">
-        <is>
-          <t xml:space="preserve">EDUU45U</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="S50">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="T50">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="U50">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="V50">
         <is>
           <t xml:space="preserve">-</t>
         </is>

</xml_diff>